<commit_message>
New Excel file added to capture loading time
</commit_message>
<xml_diff>
--- a/ExcelOutput/loadingtime.xlsx
+++ b/ExcelOutput/loadingtime.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\Projects\fms-automation\ExcelOutput\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Space\Projects\fms-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4190A1E0-8571-4338-BC0F-7D9A6416F2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1EC5D32-B92D-42EE-8654-765AEAE43DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,9 +25,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>Page Load</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sep 16</t>
   </si>
   <si>
     <t>Trucks</t>
@@ -43,6 +49,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -355,72 +362,48 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="16384" width="10.625" style="1" collapsed="1"/>
+    <col min="1" max="16384" style="1" width="9.0" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1"/>
-      <c r="C1"/>
-      <c r="D1"/>
-      <c r="E1"/>
-      <c r="F1"/>
-      <c r="G1"/>
-      <c r="H1"/>
-      <c r="I1"/>
-      <c r="J1"/>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2">
       <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2"/>
-      <c r="C2"/>
-      <c r="D2"/>
-      <c r="E2"/>
-      <c r="F2"/>
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
+        <v>3</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
+      </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3"/>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
-      <c r="F3"/>
-      <c r="G3"/>
-      <c r="H3"/>
-      <c r="I3"/>
-      <c r="J3"/>
+        <v>4</v>
+      </c>
+      <c r="B3" t="n">
+        <v>9.0</v>
+      </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4"/>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
-      <c r="F4"/>
-      <c r="G4"/>
-      <c r="H4"/>
-      <c r="I4"/>
-      <c r="J4"/>
+        <v>5</v>
+      </c>
+      <c r="B4" t="n">
+        <v>30.0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Loading time update after build success from jenkins
</commit_message>
<xml_diff>
--- a/ExcelOutput/loadingtime.xlsx
+++ b/ExcelOutput/loadingtime.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Page Load</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>Login</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sep 27</t>
   </si>
 </sst>
 </file>
@@ -362,7 +365,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -370,7 +373,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="16384" style="1" width="9.0" collapsed="false"/>
+    <col min="1" max="16384" style="1" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -380,6 +383,9 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -388,6 +394,9 @@
       <c r="B2" t="n">
         <v>1.0</v>
       </c>
+      <c r="C2" t="n">
+        <v>3.0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
@@ -396,6 +405,9 @@
       <c r="B3" t="n">
         <v>9.0</v>
       </c>
+      <c r="C3" t="n">
+        <v>5.0</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -403,6 +415,9 @@
       </c>
       <c r="B4" t="n">
         <v>30.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>2.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Vehicle Module completed and assign trailer code commented as UI changes
</commit_message>
<xml_diff>
--- a/ExcelOutput/loadingtime.xlsx
+++ b/ExcelOutput/loadingtime.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
   <si>
     <t>Page Load</t>
   </si>
@@ -45,10 +45,7 @@
     <t>Login</t>
   </si>
   <si>
-    <t xml:space="preserve"> Sep 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Sep 26</t>
+    <t xml:space="preserve"> Sep 27</t>
   </si>
 </sst>
 </file>
@@ -368,7 +365,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
@@ -389,12 +386,6 @@
       <c r="C1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -404,13 +395,7 @@
         <v>1.0</v>
       </c>
       <c r="C2" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>18.0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>29.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="3">
@@ -423,12 +408,6 @@
       <c r="C3" t="n">
         <v>5.0</v>
       </c>
-      <c r="D3" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>5.0</v>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
@@ -438,12 +417,6 @@
         <v>30.0</v>
       </c>
       <c r="C4" t="n">
-        <v>4.0</v>
-      </c>
-      <c r="D4" t="n">
-        <v>3.0</v>
-      </c>
-      <c r="E4" t="n">
         <v>2.0</v>
       </c>
     </row>

</xml_diff>